<commit_message>
definição de função de horário, inicio de implementação de função de procura de contato
</commit_message>
<xml_diff>
--- a/baseteste.xlsx
+++ b/baseteste.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/44c8030bfb8e663c/Área de Trabalho/whatappproj/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/44c8030bfb8e663c/Área de Trabalho/envio whats/span3218/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{E45ADCDC-C65C-49CA-964E-E6CAFD4D9E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6935B241-1904-49E5-9D24-E457E217E265}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{E45ADCDC-C65C-49CA-964E-E6CAFD4D9E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6F45904-BB9D-44D7-8A8C-9FD1DF50AB66}"/>
   <bookViews>
     <workbookView xWindow="1695" yWindow="2940" windowWidth="18900" windowHeight="10965" xr2:uid="{A4F5C180-A017-4115-A06C-E8222A2D5CFA}"/>
   </bookViews>
@@ -201,10 +201,10 @@
     <t>Rog gério</t>
   </si>
   <si>
-    <t>4254854445, 11982662870</t>
-  </si>
-  <si>
     <t>sergio pj</t>
+  </si>
+  <si>
+    <t>55415865, 4254854445, 11982662870</t>
   </si>
 </sst>
 </file>
@@ -1020,8 +1020,8 @@
   <sheetPr codeName="shtQuitaFacil"/>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1680,10 +1680,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
         <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Conclusão da Função procura_contato
</commit_message>
<xml_diff>
--- a/baseteste.xlsx
+++ b/baseteste.xlsx
@@ -696,10 +696,6 @@
 </externalLink>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -1020,8 +1016,8 @@
   <sheetPr codeName="shtQuitaFacil"/>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>